<commit_message>
finished all duplicate january transfer player cleaning
</commit_message>
<xml_diff>
--- a/data/league_data/england/21/england_misc.xlsx
+++ b/data/league_data/england/21/england_misc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjitvarma/Desktop/trial_git/Predicting-Football-Player-Transfer-Values/data/league_data/england/21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC7DDED-A1B8-E343-A7A0-8EA88AEED568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF9DD2-63A3-3740-8EFE-BB80681237F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1825,13 +1825,13 @@
     <t>Total Loose Balls Recovered</t>
   </si>
   <si>
-    <t>Aerial Duel Wons</t>
-  </si>
-  <si>
     <t>Aerial Duel Lost</t>
   </si>
   <si>
     <t>% Aerial Duels Won</t>
+  </si>
+  <si>
+    <t>Aerial Duel Won</t>
   </si>
 </sst>
 </file>
@@ -2699,7 +2699,7 @@
   <dimension ref="A1:X500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2794,13 +2794,13 @@
         <v>600</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>